<commit_message>
added wind2 and solar2
</commit_message>
<xml_diff>
--- a/case_input_base_190716.xlsx
+++ b/case_input_base_190716.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E54F617-D6B7-4DEE-862E-AEFA99A5FEA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2B59E1-4695-4F68-B426-AA6C27D76B53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>GLOBAL_NAME</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
   <si>
     <t>GLOBAL_NAME will be the name of the folder containing key output, name of pickle file, etc</t>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t>EIAtest3</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2877,10 +2877,10 @@
         <v>33</v>
       </c>
       <c r="B52" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="3"/>
@@ -2911,13 +2911,13 @@
     </row>
     <row r="53" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="C53" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="3"/>
@@ -2948,13 +2948,13 @@
     </row>
     <row r="54" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="C54" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="3"/>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="56" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="3"/>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="57" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57" s="15" t="b">
         <v>0</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
@@ -3090,13 +3090,13 @@
     </row>
     <row r="58" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="3"/>
@@ -3158,10 +3158,10 @@
     </row>
     <row r="60" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="13"/>
@@ -3194,77 +3194,77 @@
     <row r="61" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="16"/>
       <c r="B61" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="D61" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>52</v>
       </c>
       <c r="E61" s="17"/>
       <c r="F61" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G61" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="H61" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H61" s="18" t="s">
+      <c r="I61" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="J61" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="K61" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K61" s="18" t="s">
+      <c r="L61" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="L61" s="17" t="s">
+      <c r="M61" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="M61" s="19" t="s">
+      <c r="N61" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="N61" s="20" t="s">
+      <c r="O61" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="O61" s="18" t="s">
+      <c r="P61" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="P61" s="18" t="s">
+      <c r="Q61" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="Q61" s="21" t="s">
+      <c r="R61" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="17" t="s">
+      <c r="S61" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="S61" s="18" t="s">
+      <c r="T61" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="T61" s="17" t="s">
+      <c r="U61" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="U61" s="19" t="s">
+      <c r="V61" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="V61" s="19" t="s">
+      <c r="W61" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="W61" s="18" t="s">
+      <c r="X61" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="X61" s="17" t="s">
+      <c r="Y61" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="Y61" s="18" t="s">
+      <c r="Z61" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="Z61" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="AA61" s="17"/>
       <c r="AB61" s="17"/>
@@ -3272,14 +3272,14 @@
     </row>
     <row r="62" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" s="22">
         <v>1000000000000</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="8"/>
@@ -3309,14 +3309,14 @@
     </row>
     <row r="63" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="22">
         <v>1000000000000</v>
       </c>
       <c r="C63" s="23"/>
       <c r="D63" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="8"/>
@@ -3377,10 +3377,10 @@
     </row>
     <row r="65" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>79</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
@@ -3412,14 +3412,14 @@
     </row>
     <row r="66" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="15" t="b">
         <v>1</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="8"/>
@@ -3480,14 +3480,14 @@
     </row>
     <row r="68" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="15">
         <v>2015</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="8"/>
@@ -3517,14 +3517,14 @@
     </row>
     <row r="69" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B69" s="15">
         <v>1</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="8"/>
@@ -3554,14 +3554,14 @@
     </row>
     <row r="70" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B70" s="15">
         <v>1</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="8"/>
@@ -3591,14 +3591,14 @@
     </row>
     <row r="71" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B71" s="15">
         <v>1</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="8"/>
@@ -3628,14 +3628,14 @@
     </row>
     <row r="72" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B72" s="15">
         <v>2015</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="8"/>
@@ -3665,14 +3665,14 @@
     </row>
     <row r="73" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B73" s="15">
         <v>12</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="8"/>
@@ -3702,14 +3702,14 @@
     </row>
     <row r="74" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B74" s="15">
         <v>31</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="8"/>
@@ -3739,14 +3739,14 @@
     </row>
     <row r="75" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B75" s="15">
         <v>24</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="8"/>
@@ -3807,16 +3807,16 @@
     </row>
     <row r="77" spans="1:29" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77" s="15">
         <v>0</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="8"/>
@@ -3877,10 +3877,10 @@
     </row>
     <row r="79" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="4"/>
@@ -3912,17 +3912,17 @@
     </row>
     <row r="80" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80" s="32">
         <f>N80</f>
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C80" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="8">
@@ -3976,17 +3976,17 @@
     </row>
     <row r="81" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81" s="22">
         <f>Z81</f>
         <v>1E-8</v>
       </c>
       <c r="C81" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D81" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="D81" s="36" t="s">
-        <v>101</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="8"/>
@@ -4044,16 +4044,16 @@
     </row>
     <row r="82" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B82" s="15">
         <v>0</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D82" t="s">
         <v>103</v>
-      </c>
-      <c r="D82" t="s">
-        <v>104</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="8"/>
@@ -4083,16 +4083,16 @@
     </row>
     <row r="83" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B83" s="15">
         <v>0</v>
       </c>
       <c r="C83" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" t="s">
         <v>106</v>
-      </c>
-      <c r="D83" t="s">
-        <v>107</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="8"/>
@@ -4153,10 +4153,10 @@
     </row>
     <row r="85" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B85" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -4188,17 +4188,17 @@
     </row>
     <row r="86" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B86" s="32">
         <f>N86</f>
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="8">
@@ -4252,17 +4252,17 @@
     </row>
     <row r="87" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B87" s="22">
         <f>Z87</f>
         <v>1.05E-8</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="D87" s="36" t="s">
-        <v>101</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="8"/>
@@ -4320,16 +4320,16 @@
     </row>
     <row r="88" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B88" s="15">
         <v>0</v>
       </c>
       <c r="C88" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="8"/>
@@ -4359,16 +4359,16 @@
     </row>
     <row r="89" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B89" s="15">
         <v>0</v>
       </c>
       <c r="C89" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="8"/>
@@ -4429,14 +4429,14 @@
     </row>
     <row r="91" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B91" s="32">
         <f>N91</f>
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
@@ -4491,14 +4491,14 @@
     </row>
     <row r="92" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B92" s="22">
         <f>Z92</f>
         <v>3.8992074681058302E-2</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
@@ -4560,16 +4560,16 @@
     </row>
     <row r="93" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B93" s="15">
         <v>0</v>
       </c>
       <c r="C93" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="8"/>
@@ -4599,16 +4599,16 @@
     </row>
     <row r="94" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B94" s="40">
         <v>0.46100000000000002</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="8"/>
@@ -4669,14 +4669,14 @@
     </row>
     <row r="96" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B96" s="32">
         <f>N96</f>
         <v>2.7271220888813726E-2</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
@@ -4731,14 +4731,14 @@
     </row>
     <row r="97" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B97" s="22">
         <f>Z97</f>
         <v>5.6563468785905562E-2</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
@@ -4800,16 +4800,16 @@
     </row>
     <row r="98" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B98" s="15">
         <v>0</v>
       </c>
       <c r="C98" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="8"/>
@@ -4839,16 +4839,16 @@
     </row>
     <row r="99" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B99" s="40">
         <v>0.16700000000000001</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="8"/>
@@ -4909,17 +4909,17 @@
     </row>
     <row r="101" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B101" s="32">
         <f>N101</f>
         <v>6.4753901191501415E-2</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D101" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="8">
@@ -4968,24 +4968,24 @@
       <c r="Y101" s="31"/>
       <c r="Z101" s="43"/>
       <c r="AA101" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB101" s="4"/>
       <c r="AC101" s="4"/>
     </row>
     <row r="102" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B102" s="22">
         <f>Z102</f>
         <v>2.2838149285310763E-2</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D102" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="8"/>
@@ -5041,23 +5041,23 @@
         <v>2.2838149285310763E-2</v>
       </c>
       <c r="AA102" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB102" s="4"/>
       <c r="AC102" s="4"/>
     </row>
     <row r="103" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B103" s="15">
         <v>0</v>
       </c>
       <c r="C103" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D103" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="8"/>
@@ -5087,16 +5087,16 @@
     </row>
     <row r="104" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B104" s="15">
         <v>0</v>
       </c>
       <c r="C104" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="8"/>
@@ -5157,17 +5157,17 @@
     </row>
     <row r="106" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B106" s="32">
         <f>N106</f>
         <v>4.2392529406082022E-3</v>
       </c>
       <c r="C106" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="8">
@@ -5218,14 +5218,14 @@
     </row>
     <row r="107" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B107" s="22">
         <f t="shared" ref="B107:B108" si="0">Z107</f>
         <v>0</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="4"/>
@@ -5272,14 +5272,14 @@
     </row>
     <row r="108" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B108" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
@@ -5326,14 +5326,14 @@
     </row>
     <row r="109" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B109" s="15">
         <v>0.9</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="8"/>
@@ -5363,17 +5363,17 @@
     </row>
     <row r="110" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B110" s="32">
         <f>1.01^(1/HOURS_PER_YEAR)-1</f>
         <v>1.1351290010175319E-6</v>
       </c>
       <c r="C110" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="E110" s="9" t="str">
         <f>HYPERLINK("https://batteryuniversity.com/learn/article/elevating_self_discharge","Buchmann, 2018, Battery University")</f>
@@ -5406,17 +5406,17 @@
     </row>
     <row r="111" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B111" s="40">
         <f>1568/261</f>
         <v>6.0076628352490422</v>
       </c>
       <c r="C111" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="8"/>
@@ -5477,17 +5477,17 @@
     </row>
     <row r="113" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B113" s="45">
         <f t="shared" ref="B113:B115" si="3">N113</f>
         <v>3.2304881600325706E-6</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="8">
@@ -5501,7 +5501,7 @@
         <v>20</v>
       </c>
       <c r="I113" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J113" s="33">
         <f>DISCOUNT_RATE*(1+DISCOUNT_RATE)^H113/((1+DISCOUNT_RATE)^H113-1)</f>
@@ -5537,14 +5537,14 @@
     </row>
     <row r="114" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B114" s="45">
         <f t="shared" si="3"/>
         <v>1.184512325345276E-2</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="4"/>
@@ -5559,7 +5559,7 @@
         <v>20</v>
       </c>
       <c r="I114" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J114" s="33">
         <f>DISCOUNT_RATE*(1+DISCOUNT_RATE)^H114/((1+DISCOUNT_RATE)^H114-1)</f>
@@ -5595,14 +5595,14 @@
     </row>
     <row r="115" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B115" s="45">
         <f t="shared" si="3"/>
         <v>4.9534151787166088E-2</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="4"/>
@@ -5617,7 +5617,7 @@
         <v>20</v>
       </c>
       <c r="I115" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J115" s="33">
         <f>DISCOUNT_RATE*(1+DISCOUNT_RATE)^H115/((1+DISCOUNT_RATE)^H115-1)</f>
@@ -5653,14 +5653,14 @@
     </row>
     <row r="116" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B116" s="22">
         <f t="shared" ref="B116:B117" si="6">Z116</f>
         <v>0</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="4"/>
@@ -5707,14 +5707,14 @@
     </row>
     <row r="117" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B117" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="4"/>
@@ -5761,17 +5761,17 @@
     </row>
     <row r="118" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B118" s="48">
         <f>1.0001^(1/HOURS_PER_YEAR)-1</f>
         <v>1.1407375488659E-8</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E118" s="9" t="str">
         <f>HYPERLINK("http://juser.fz-juelich.de/record/135790/files/Energie%26Umwelt_78-04.pdf","Crotogino et al., 2010, p43")</f>
@@ -5804,7 +5804,7 @@
     </row>
     <row r="119" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B119" s="48">
         <v>0.3</v>
@@ -5873,109 +5873,109 @@
     </row>
     <row r="121" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B121" s="59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
     </row>
     <row r="122" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B122" s="60">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C122" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D122" s="57">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="E122" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" s="52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B123" s="60">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C123" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D123" s="58"/>
       <c r="E123" s="58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="124" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A124" s="52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B124" s="61">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C124" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D124" s="58"/>
     </row>
     <row r="125" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B125" s="61">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C125" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D125" s="58"/>
     </row>
     <row r="126" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B126" s="59">
         <v>0.1</v>
       </c>
       <c r="C126" s="58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E126" s="53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="127" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B127" s="59">
         <v>1</v>
       </c>
       <c r="C127" s="58"/>
       <c r="D127" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="128" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B128" s="15">
         <v>10</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="4"/>
@@ -6039,7 +6039,7 @@
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="3"/>
@@ -6101,103 +6101,103 @@
     </row>
     <row r="132" spans="1:29" s="49" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="B132" s="50" t="s">
         <v>152</v>
-      </c>
-      <c r="B132" s="50" t="s">
-        <v>153</v>
       </c>
       <c r="C132" s="51"/>
     </row>
     <row r="133" spans="1:29" s="52" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B133" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C133" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D133" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E133" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E133" s="52" t="s">
-        <v>88</v>
-      </c>
       <c r="F133" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G133" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H133" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I133" s="52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J133" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="K133" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="K133" s="52" t="s">
-        <v>116</v>
-      </c>
       <c r="L133" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="M133" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="M133" s="52" t="s">
-        <v>121</v>
-      </c>
       <c r="N133" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O133" s="52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P133" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q133" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="R133" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="R133" s="52" t="s">
-        <v>136</v>
-      </c>
       <c r="S133" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T133" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="U133" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="U133" s="52" t="s">
+      <c r="V133" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="V133" s="52" t="s">
+      <c r="W133" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="W133" s="52" t="s">
-        <v>148</v>
-      </c>
       <c r="X133" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y133" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="Y133" s="52" t="s">
+      <c r="Z133" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="Z133" s="52" t="s">
+      <c r="AA133" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="AA133" s="52" t="s">
-        <v>160</v>
-      </c>
       <c r="AB133" s="52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="134" spans="1:29" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="135" spans="1:29" s="54" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B135" s="54">
         <v>2015</v>
@@ -6283,7 +6283,7 @@
     </row>
     <row r="136" spans="1:29" s="54" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A136" s="54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B136" s="54">
         <v>2015</v>
@@ -6295,7 +6295,7 @@
         <v>2015</v>
       </c>
       <c r="E136" s="54">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F136" s="54">
         <v>0.25600000000000001</v>
@@ -6369,7 +6369,7 @@
     </row>
     <row r="137" spans="1:29" s="54" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" s="54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B137" s="54">
         <v>2015</v>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="138" spans="1:29" s="55" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B138" s="55">
         <v>2015</v>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="140" spans="1:29" s="49" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B140" s="50"/>
     </row>

</xml_diff>